<commit_message>
Batch running mid night and insert data from excel file
</commit_message>
<xml_diff>
--- a/src/main/resources/birthdays.xlsx
+++ b/src/main/resources/birthdays.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\Java Development\2025\April\Birthday-Notification\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{137DDA0B-DF03-40F5-A58B-8B29ED591451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C909E6E4-207B-4486-9E45-BC2716B6238E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B3D5649A-E3BC-4F7B-A1F9-AD3442945DC6}"/>
   </bookViews>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
-    <t>ID</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -63,6 +60,9 @@
   </si>
   <si>
     <t>dfjdjJKGJJBKJKjlkdhfjkgdhkj983457843dbffdj</t>
+  </si>
+  <si>
+    <t>S NO</t>
   </si>
 </sst>
 </file>
@@ -455,9 +455,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48B9B603-79D7-40F1-B26C-3E4DA3FD3424}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
@@ -470,22 +468,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -493,19 +491,19 @@
         <v>1903</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" s="1">
         <v>33013</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2">
         <v>98985679857</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Get birthday from database and send notification successfully(Email)
</commit_message>
<xml_diff>
--- a/src/main/resources/birthdays.xlsx
+++ b/src/main/resources/birthdays.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\Java Development\2025\April\Birthday-Notification\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C909E6E4-207B-4486-9E45-BC2716B6238E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6167D4E2-74F2-4D72-9ED9-58271B92260E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B3D5649A-E3BC-4F7B-A1F9-AD3442945DC6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Name</t>
   </si>
@@ -63,6 +63,15 @@
   </si>
   <si>
     <t>S NO</t>
+  </si>
+  <si>
+    <t>Alina</t>
+  </si>
+  <si>
+    <t>akis441981@gmail.com</t>
+  </si>
+  <si>
+    <t>fknvbckjbnkcjFHFHGFkhkjhkjhkj76576jdfkjdh</t>
   </si>
 </sst>
 </file>
@@ -453,9 +462,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48B9B603-79D7-40F1-B26C-3E4DA3FD3424}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
@@ -494,7 +505,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="1">
-        <v>33013</v>
+        <v>32970</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>6</v>
@@ -504,13 +515,34 @@
       </c>
       <c r="F2" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <v>1904</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1">
+        <v>36623</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>87465487887</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{4FC98B77-2E8C-4A8A-887D-A402F21926C7}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{C0FB9247-DBEA-46F9-B5F3-3FE74A663152}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
No duplicate data stored
</commit_message>
<xml_diff>
--- a/src/main/resources/birthdays.xlsx
+++ b/src/main/resources/birthdays.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\Java Development\2025\April\Birthday-Notification\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6167D4E2-74F2-4D72-9ED9-58271B92260E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F67BCB-2169-42EE-8907-151B67891FDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B3D5649A-E3BC-4F7B-A1F9-AD3442945DC6}"/>
   </bookViews>
@@ -462,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48B9B603-79D7-40F1-B26C-3E4DA3FD3424}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -537,6 +537,15 @@
         <v>11</v>
       </c>
     </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <v>1905</v>
+      </c>
+      <c r="C4" s="1">
+        <v>36988</v>
+      </c>
+      <c r="D4" s="3"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{4FC98B77-2E8C-4A8A-887D-A402F21926C7}"/>

</xml_diff>

<commit_message>
Now we can send notification based on event and message will pick up randomly based on event and no duplicate send each person when batch is run
</commit_message>
<xml_diff>
--- a/src/main/resources/birthdays.xlsx
+++ b/src/main/resources/birthdays.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\Java Development\2025\April\Birthday-Notification\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F67BCB-2169-42EE-8907-151B67891FDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{873F137E-0A41-4961-8477-09B9CA8B2D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B3D5649A-E3BC-4F7B-A1F9-AD3442945DC6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Name</t>
   </si>
@@ -72,6 +72,18 @@
   </si>
   <si>
     <t>fknvbckjbnkcjFHFHGFkhkjhkjhkj76576jdfkjdh</t>
+  </si>
+  <si>
+    <t>deendayal555kumawat@gmail.com</t>
+  </si>
+  <si>
+    <t>Iron Man</t>
+  </si>
+  <si>
+    <t>user221user@gmail.com</t>
+  </si>
+  <si>
+    <t>Captain America</t>
   </si>
 </sst>
 </file>
@@ -462,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48B9B603-79D7-40F1-B26C-3E4DA3FD3424}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -541,17 +553,50 @@
       <c r="A4">
         <v>1905</v>
       </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
       <c r="C4" s="1">
         <v>36988</v>
       </c>
-      <c r="D4" s="3"/>
+      <c r="D4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4">
+        <v>7648648887</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>1906</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1">
+        <v>36624</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5">
+        <v>87674876845</v>
+      </c>
+      <c r="F5" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{4FC98B77-2E8C-4A8A-887D-A402F21926C7}"/>
     <hyperlink ref="D3" r:id="rId2" xr:uid="{C0FB9247-DBEA-46F9-B5F3-3FE74A663152}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{BD669A09-E5D9-4F06-892F-5FF00E0E7CA8}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{96E8B561-4E13-4A7D-BD96-37305931A635}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat(config): add environment-specific properties for local and Docker
- Created application-local.properties for local development
- Created application-docker.properties for Docker environment
- Externalized Excel file path and datasource URL based on active profile
- Added support for SPRING_PROFILES_ACTIVE to switch between environments
</commit_message>
<xml_diff>
--- a/src/main/resources/birthdays.xlsx
+++ b/src/main/resources/birthdays.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\Java Development\2025\April\Birthday-Notification\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{873F137E-0A41-4961-8477-09B9CA8B2D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB4A6C3-AB77-4ECA-B661-37D1F9DC4898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B3D5649A-E3BC-4F7B-A1F9-AD3442945DC6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>Name</t>
   </si>
@@ -59,9 +59,6 @@
     <t>kkumawat1111@gmail.com</t>
   </si>
   <si>
-    <t>dfjdjJKGJJBKJKjlkdhfjkgdhkj983457843dbffdj</t>
-  </si>
-  <si>
     <t>S NO</t>
   </si>
   <si>
@@ -71,9 +68,6 @@
     <t>akis441981@gmail.com</t>
   </si>
   <si>
-    <t>fknvbckjbnkcjFHFHGFkhkjhkjhkj76576jdfkjdh</t>
-  </si>
-  <si>
     <t>deendayal555kumawat@gmail.com</t>
   </si>
   <si>
@@ -84,6 +78,9 @@
   </si>
   <si>
     <t>Captain America</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -477,7 +474,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -491,7 +488,7 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -526,7 +523,7 @@
         <v>98985679857</v>
       </c>
       <c r="F2" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -534,19 +531,19 @@
         <v>1904</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1">
         <v>36623</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3">
         <v>87465487887</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -554,19 +551,19 @@
         <v>1905</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1">
         <v>36988</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E4">
         <v>7648648887</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -574,19 +571,19 @@
         <v>1906</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1">
         <v>36624</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E5">
         <v>87674876845</v>
       </c>
       <c r="F5" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>